<commit_message>
Added extent report logs in Test Classes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridMultiThreadedFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridMultiThreadedFrameworkTestDriver.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridMultiThreadedProjectTemplate\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niraj Tiwari\eclipse-workspace\HybridMultiThreadedProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF35386-F29B-4AD2-8D21-1A80752C7357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A8E8F1-5165-4607-A1E2-525259ED51BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="88">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -89,83 +89,178 @@
     <t>User2</t>
   </si>
   <si>
+    <t>LoginType</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>ExpSearchText</t>
+  </si>
+  <si>
+    <t>What do you want to learn?</t>
+  </si>
+  <si>
+    <t>User3</t>
+  </si>
+  <si>
+    <t>User4</t>
+  </si>
+  <si>
+    <t>User5</t>
+  </si>
+  <si>
+    <t>TC_0002_1</t>
+  </si>
+  <si>
+    <t>TC_0002_2</t>
+  </si>
+  <si>
+    <t>TC_0002_3</t>
+  </si>
+  <si>
+    <t>TC_0002_4</t>
+  </si>
+  <si>
+    <t>TC_0002_5</t>
+  </si>
+  <si>
+    <t>notadmin</t>
+  </si>
+  <si>
+    <t>notpassword</t>
+  </si>
+  <si>
+    <t>password125</t>
+  </si>
+  <si>
+    <t>Invalid user name or password</t>
+  </si>
+  <si>
+    <t>ExpErrorMessage</t>
+  </si>
+  <si>
+    <t>NegativeLoginScenarios</t>
+  </si>
+  <si>
+    <t>HomePageFeatures</t>
+  </si>
+  <si>
+    <t>CoursePageDetails</t>
+  </si>
+  <si>
+    <t>SearchPageFeatures</t>
+  </si>
+  <si>
+    <t>JavaSearchFunctionality</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>CoursePage</t>
+  </si>
+  <si>
+    <t>SearchPage</t>
+  </si>
+  <si>
+    <t>JavaSearch</t>
+  </si>
+  <si>
+    <t>TC_0003_1</t>
+  </si>
+  <si>
+    <t>TC_0004_1</t>
+  </si>
+  <si>
+    <t>TC_0005_1</t>
+  </si>
+  <si>
+    <t>TC_0006_1</t>
+  </si>
+  <si>
+    <t>ExpHomePageHeader</t>
+  </si>
+  <si>
+    <t>ExpHomePageDesc</t>
+  </si>
+  <si>
+    <t>The technology
+learning platform</t>
+  </si>
+  <si>
+    <t>Keep up with technology with expert-led courses, assessments and tools that help you build the skills you need, when you need them.
+For organizations, get unprecedented insight into skills strengths and weaknesses and align learning to what matters.</t>
+  </si>
+  <si>
+    <t>CourseName</t>
+  </si>
+  <si>
+    <t>Java Fundamentals: The Java Language</t>
+  </si>
+  <si>
+    <t>ExpCourseOverviewText</t>
+  </si>
+  <si>
+    <t>ExpFreeTrailText</t>
+  </si>
+  <si>
+    <t>ExpCourseHeaderText</t>
+  </si>
+  <si>
+    <t>ExpCourseDescriptionText</t>
+  </si>
+  <si>
+    <t>This course provides thorough coverage of the core Java platform, giving you the skills needed to begin developing in the Java Runtime Environment (JRE) and serving as a solid foundation for all Java-based development environments.</t>
+  </si>
+  <si>
+    <t>Start a FREE 10-day trial</t>
+  </si>
+  <si>
+    <t>Play course overview</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>TC_0001_2</t>
+  </si>
+  <si>
+    <t>TC_0005_2</t>
+  </si>
+  <si>
+    <t>TC_0004_2</t>
+  </si>
+  <si>
+    <t>TC_0003_2</t>
+  </si>
+  <si>
+    <t>TC_0006_2</t>
+  </si>
+  <si>
+    <t>https://nirajt03.github.io/sample-website/</t>
+  </si>
+  <si>
+    <t>test.admin</t>
+  </si>
+  <si>
+    <t>test.user</t>
+  </si>
+  <si>
+    <t>pragyan@123</t>
+  </si>
+  <si>
     <r>
-      <t>verify</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>LoginFunctionality</t>
-    </r>
-  </si>
-  <si>
-    <t>LoginType</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>password123</t>
-  </si>
-  <si>
-    <t>ExpSearchText</t>
-  </si>
-  <si>
-    <t>What do you want to learn?</t>
-  </si>
-  <si>
-    <t>User3</t>
-  </si>
-  <si>
-    <t>User4</t>
-  </si>
-  <si>
-    <t>User5</t>
-  </si>
-  <si>
-    <t>TC_0002_1</t>
-  </si>
-  <si>
-    <t>TC_0002_2</t>
-  </si>
-  <si>
-    <t>TC_0002_3</t>
-  </si>
-  <si>
-    <t>TC_0002_4</t>
-  </si>
-  <si>
-    <t>TC_0002_5</t>
-  </si>
-  <si>
-    <t>notadmin</t>
-  </si>
-  <si>
-    <t>notpassword</t>
-  </si>
-  <si>
-    <t>password125</t>
-  </si>
-  <si>
-    <t>Invalid user name or password</t>
-  </si>
-  <si>
-    <t>ExpErrorMessage</t>
-  </si>
-  <si>
-    <r>
-      <t>verify</t>
+      <t>Test</t>
     </r>
     <r>
       <rPr>
@@ -175,21 +270,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>LoginPageNegative</t>
+      <t>LoginPage</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Scenarios</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>verify</t>
+      <t>Test</t>
     </r>
     <r>
       <rPr>
@@ -199,21 +285,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>HomePage</t>
+      <t>LoginPageNegativeScenarios</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Features</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>verify</t>
+      <t>Test</t>
     </r>
     <r>
       <rPr>
@@ -223,21 +300,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>CoursePage</t>
+      <t>HomePageFeatures</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Features</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>verify</t>
+      <t>Test</t>
     </r>
     <r>
       <rPr>
@@ -247,21 +315,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>SearchPage</t>
+      <t>CoursePageFeatures</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Features</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>verify</t>
+      <t>Test</t>
     </r>
     <r>
       <rPr>
@@ -271,127 +330,47 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>JavaSearch</t>
+      <t>SearchPageFeatures</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Test</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Functionality</t>
+      <t>JavaSearchFunctionality</t>
     </r>
   </si>
   <si>
-    <t>NegativeLoginScenarios</t>
-  </si>
-  <si>
-    <t>HomePageFeatures</t>
-  </si>
-  <si>
-    <t>CoursePageDetails</t>
-  </si>
-  <si>
-    <t>SearchPageFeatures</t>
-  </si>
-  <si>
-    <t>JavaSearchFunctionality</t>
-  </si>
-  <si>
-    <t>HomePage</t>
-  </si>
-  <si>
-    <t>CoursePage</t>
-  </si>
-  <si>
-    <t>SearchPage</t>
-  </si>
-  <si>
-    <t>JavaSearch</t>
-  </si>
-  <si>
-    <t>TC_0003_1</t>
-  </si>
-  <si>
-    <t>TC_0004_1</t>
-  </si>
-  <si>
-    <t>TC_0005_1</t>
-  </si>
-  <si>
-    <t>TC_0006_1</t>
-  </si>
-  <si>
-    <t>ExpHomePageHeader</t>
-  </si>
-  <si>
-    <t>ExpHomePageDesc</t>
-  </si>
-  <si>
-    <t>The technology
-learning platform</t>
-  </si>
-  <si>
-    <t>Keep up with technology with expert-led courses, assessments and tools that help you build the skills you need, when you need them.
-For organizations, get unprecedented insight into skills strengths and weaknesses and align learning to what matters.</t>
-  </si>
-  <si>
-    <t>CourseName</t>
-  </si>
-  <si>
-    <t>Java Fundamentals: The Java Language</t>
-  </si>
-  <si>
-    <t>ExpCourseOverviewText</t>
-  </si>
-  <si>
-    <t>ExpFreeTrailText</t>
-  </si>
-  <si>
-    <t>ExpCourseHeaderText</t>
-  </si>
-  <si>
-    <t>ExpCourseDescriptionText</t>
-  </si>
-  <si>
-    <t>This course provides thorough coverage of the core Java platform, giving you the skills needed to begin developing in the Java Runtime Environment (JRE) and serving as a solid foundation for all Java-based development environments.</t>
-  </si>
-  <si>
-    <t>Start a FREE 10-day trial</t>
-  </si>
-  <si>
-    <t>Play course overview</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>TC_0001_2</t>
-  </si>
-  <si>
-    <t>TC_0005_2</t>
-  </si>
-  <si>
-    <t>TC_0004_2</t>
-  </si>
-  <si>
-    <t>TC_0003_2</t>
-  </si>
-  <si>
-    <t>TC_0006_2</t>
-  </si>
-  <si>
-    <t>https://nirajt03.github.io/sample-website/</t>
-  </si>
-  <si>
-    <t>test.admin</t>
-  </si>
-  <si>
-    <t>test.user</t>
-  </si>
-  <si>
-    <t>pragyan@123</t>
+    <t>ManualTCIDs</t>
+  </si>
+  <si>
+    <t>TCs-001,TCs-002,TCs-003</t>
+  </si>
+  <si>
+    <t>TCs-003,TCs-004,TCs-005</t>
+  </si>
+  <si>
+    <t>TCs-006,TCs-007,TCs-008,TCs-008</t>
+  </si>
+  <si>
+    <t>TCs-008,TCs-009,TCs-010,TCs-011</t>
+  </si>
+  <si>
+    <t>TCs-012,TCs-013,TCs-014,TCs-015</t>
+  </si>
+  <si>
+    <t>TCs-012,TCs-013,TCs-014,TCs-016</t>
+  </si>
+  <si>
+    <t>TCs-016,TCs-017,TCs-018,TCs-019,TCs-020</t>
   </si>
 </sst>
 </file>
@@ -401,7 +380,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,13 +436,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -503,7 +475,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +523,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -708,17 +686,17 @@
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
+    <xf numFmtId="43" fontId="8" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -752,7 +730,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -761,7 +739,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -802,9 +780,18 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1101,18 +1088,18 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1134,13 +1121,13 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1148,19 +1135,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
     </row>
@@ -1182,18 +1169,18 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1207,12 +1194,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>14</v>
@@ -1221,74 +1208,74 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>48</v>
-      </c>
       <c r="D7" s="24" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1312,23 +1299,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.46484375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1336,7 +1324,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>11</v>
@@ -1345,10 +1333,13 @@
         <v>13</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
@@ -1356,40 +1347,46 @@
         <v>12</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"TC_0001_1,Not To Run"</formula1>
@@ -1402,22 +1399,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E7E38D-2134-4D7B-AFCC-79142EC6D7FA}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1431,88 +1429,106 @@
         <v>13</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>37</v>
+      <c r="F6" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6" xr:uid="{46613FB6-A1FF-4C4B-869E-F63249A03F3F}">
       <formula1>"TC_0002_1,Not To Run"</formula1>
@@ -1524,24 +1540,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B881C555-7FA8-4DD1-A7D0-F5D26883CF57}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="36.06640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.46484375" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.44140625" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1549,78 +1566,87 @@
         <v>10</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="54" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>68</v>
-      </c>
       <c r="H2" s="37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="54" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>68</v>
-      </c>
       <c r="H3" s="36" t="s">
-        <v>69</v>
+        <v>63</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{8DD5F003-84F9-4453-B61D-C6EE61EACE70}">
       <formula1>"TC_0003_1,Not To Run"</formula1>
@@ -1632,22 +1658,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3356B94C-5B4C-4FFF-9F00-EBBCCEB4F868}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.59765625" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.5546875" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>15</v>
       </c>
@@ -1655,51 +1682,60 @@
         <v>10</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="54" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="54" x14ac:dyDescent="0.45">
+      <c r="F2" s="36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{CE3AAC6A-F7EC-495F-A000-D9D096D0025F}">
       <formula1>"TC_0004_1,Not To Run"</formula1>
@@ -1712,21 +1748,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8C79C5-CBC0-4DDF-9AC8-C72E09C8FEF2}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1734,42 +1771,51 @@
         <v>10</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{2EB08E7A-9DE2-4D6F-A588-CBA4DB251774}">
       <formula1>"TC_0005_1,Not To Run"</formula1>
@@ -1781,22 +1827,23 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B62C1C-0C0C-47DD-9D4A-D15FCE655D45}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G1" sqref="G1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="36.06640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.53125" style="34" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.5546875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1804,60 +1851,69 @@
         <v>10</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="40.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>62</v>
-      </c>
       <c r="E2" s="36" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="40.5" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{7EE091FA-9632-4F03-8BD6-6DF4BEE70883}">
       <formula1>"TC_0006_1,Not To Run"</formula1>

</xml_diff>